<commit_message>
stop tracking dev-specific configs.
</commit_message>
<xml_diff>
--- a/Documentation/wiring.xlsx
+++ b/Documentation/wiring.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37608" windowHeight="13584" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37608" windowHeight="13572" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wires" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="178">
   <si>
     <t>Wire Number</t>
   </si>
@@ -234,9 +234,6 @@
     <t>DIN rail</t>
   </si>
   <si>
-    <t>10"</t>
-  </si>
-  <si>
     <t>8"</t>
   </si>
   <si>
@@ -276,9 +273,6 @@
     <t>Automation Direct</t>
   </si>
   <si>
-    <t>wire tray</t>
-  </si>
-  <si>
     <t>Green terminal block</t>
   </si>
   <si>
@@ -321,9 +315,6 @@
     <t>1" wide, 1.5" high, 12" long</t>
   </si>
   <si>
-    <t>1" wide, 1.5" high, 8" long</t>
-  </si>
-  <si>
     <t>T1E-1015G-1</t>
   </si>
   <si>
@@ -427,6 +418,147 @@
   </si>
   <si>
     <t>20"×16.1"×7.9"</t>
+  </si>
+  <si>
+    <t>T3-1L</t>
+  </si>
+  <si>
+    <t>T3-2L</t>
+  </si>
+  <si>
+    <t>T3-3L</t>
+  </si>
+  <si>
+    <t>T3-4L</t>
+  </si>
+  <si>
+    <t>T3-5L</t>
+  </si>
+  <si>
+    <t>T3-6L</t>
+  </si>
+  <si>
+    <t>T3-1U</t>
+  </si>
+  <si>
+    <t>T3-2U</t>
+  </si>
+  <si>
+    <t>T3-3U</t>
+  </si>
+  <si>
+    <t>T3-4U</t>
+  </si>
+  <si>
+    <t>T3-5U</t>
+  </si>
+  <si>
+    <t>T3-6U</t>
+  </si>
+  <si>
+    <t>T3-7L</t>
+  </si>
+  <si>
+    <t>4-20mA</t>
+  </si>
+  <si>
+    <t>dry contact</t>
+  </si>
+  <si>
+    <t>T3-8L</t>
+  </si>
+  <si>
+    <t>T3-10L</t>
+  </si>
+  <si>
+    <t>T3-9L</t>
+  </si>
+  <si>
+    <t>1" wide, 1.5" high, 10" long</t>
+  </si>
+  <si>
+    <t>T3-7U</t>
+  </si>
+  <si>
+    <t>232U</t>
+  </si>
+  <si>
+    <t>T3-8U</t>
+  </si>
+  <si>
+    <t>233U</t>
+  </si>
+  <si>
+    <t>T3-9U</t>
+  </si>
+  <si>
+    <t>234U</t>
+  </si>
+  <si>
+    <t>T3-10U</t>
+  </si>
+  <si>
+    <t>235U</t>
+  </si>
+  <si>
+    <t>235L</t>
+  </si>
+  <si>
+    <t>234L</t>
+  </si>
+  <si>
+    <t>233L</t>
+  </si>
+  <si>
+    <t>232L</t>
+  </si>
+  <si>
+    <t>231U</t>
+  </si>
+  <si>
+    <t>230U</t>
+  </si>
+  <si>
+    <t>229U</t>
+  </si>
+  <si>
+    <t>228U</t>
+  </si>
+  <si>
+    <t>227U</t>
+  </si>
+  <si>
+    <t>226U</t>
+  </si>
+  <si>
+    <t>wire duct</t>
+  </si>
+  <si>
+    <t>CT-VOLTS-POS</t>
+  </si>
+  <si>
+    <t>CT-VOLTS-NEG</t>
+  </si>
+  <si>
+    <t>120L</t>
+  </si>
+  <si>
+    <t>120N</t>
+  </si>
+  <si>
+    <t>CT-RS485-NEG</t>
+  </si>
+  <si>
+    <t>CT-RS405-POS</t>
+  </si>
+  <si>
+    <t>CT-PWR-GND</t>
+  </si>
+  <si>
+    <t>CT-PWR-POS</t>
+  </si>
+  <si>
+    <t>10.5"</t>
   </si>
 </sst>
 </file>
@@ -862,15 +994,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -938,7 +1072,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -957,6 +1091,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>104</v>
+      </c>
       <c r="B5" s="1">
         <v>213</v>
       </c>
@@ -977,7 +1114,12 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="B6" s="1">
+        <v>107</v>
+      </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
@@ -995,6 +1137,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>106</v>
+      </c>
       <c r="B7" s="1">
         <v>108</v>
       </c>
@@ -1015,6 +1160,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>107</v>
+      </c>
       <c r="B8">
         <v>210</v>
       </c>
@@ -1035,6 +1183,9 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>108</v>
+      </c>
       <c r="B9">
         <v>211</v>
       </c>
@@ -1055,6 +1206,9 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>109</v>
+      </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -1072,6 +1226,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>110</v>
+      </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -1089,6 +1246,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>111</v>
+      </c>
       <c r="B12" t="s">
         <v>27</v>
       </c>
@@ -1112,6 +1272,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>112</v>
+      </c>
       <c r="B13" t="s">
         <v>35</v>
       </c>
@@ -1135,6 +1298,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>113</v>
+      </c>
       <c r="B14" t="s">
         <v>28</v>
       </c>
@@ -1158,6 +1324,9 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>114</v>
+      </c>
       <c r="B15" t="s">
         <v>32</v>
       </c>
@@ -1181,6 +1350,9 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>115</v>
+      </c>
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -1199,8 +1371,14 @@
       <c r="G16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>116</v>
+      </c>
       <c r="B17">
         <v>105</v>
       </c>
@@ -1210,11 +1388,20 @@
       <c r="D17">
         <v>8.5</v>
       </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
       <c r="G17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>117</v>
+      </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
@@ -1224,11 +1411,20 @@
       <c r="D18">
         <v>5</v>
       </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
       <c r="G18" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>118</v>
+      </c>
       <c r="B19" t="s">
         <v>42</v>
       </c>
@@ -1238,11 +1434,20 @@
       <c r="D19">
         <v>5</v>
       </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
       <c r="G19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>119</v>
+      </c>
       <c r="B20" t="s">
         <v>44</v>
       </c>
@@ -1252,11 +1457,20 @@
       <c r="D20">
         <v>5</v>
       </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
       <c r="G20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>120</v>
+      </c>
       <c r="B21">
         <v>236</v>
       </c>
@@ -1266,11 +1480,23 @@
       <c r="D21">
         <v>5</v>
       </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>31</v>
+      </c>
       <c r="G21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>121</v>
+      </c>
       <c r="B22" t="s">
         <v>46</v>
       </c>
@@ -1280,11 +1506,23 @@
       <c r="D22">
         <v>3.5</v>
       </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>31</v>
+      </c>
       <c r="G22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>122</v>
+      </c>
       <c r="B23" t="s">
         <v>47</v>
       </c>
@@ -1294,11 +1532,23 @@
       <c r="D23">
         <v>3.5</v>
       </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
+        <v>31</v>
+      </c>
       <c r="G23" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>123</v>
+      </c>
       <c r="B24" t="s">
         <v>48</v>
       </c>
@@ -1308,11 +1558,23 @@
       <c r="D24">
         <v>3.5</v>
       </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>31</v>
+      </c>
       <c r="G24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>124</v>
+      </c>
       <c r="B25" t="s">
         <v>49</v>
       </c>
@@ -1322,11 +1584,23 @@
       <c r="D25">
         <v>3.5</v>
       </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>31</v>
+      </c>
       <c r="G25" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>125</v>
+      </c>
       <c r="B26" t="s">
         <v>50</v>
       </c>
@@ -1336,28 +1610,908 @@
       <c r="D26">
         <v>3.5</v>
       </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>31</v>
+      </c>
       <c r="G26" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="H26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>126</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27">
+        <v>225</v>
+      </c>
+      <c r="D27">
+        <v>6.5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>127</v>
+      </c>
+      <c r="B28">
+        <v>225</v>
+      </c>
+      <c r="C28">
+        <v>222</v>
+      </c>
+      <c r="D28">
+        <v>5.5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>128</v>
+      </c>
+      <c r="B29">
+        <v>222</v>
+      </c>
+      <c r="C29">
+        <v>219</v>
+      </c>
+      <c r="D29">
+        <v>5.5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>129</v>
+      </c>
+      <c r="B30">
+        <v>219</v>
+      </c>
+      <c r="C30">
+        <v>216</v>
+      </c>
+      <c r="D30">
+        <v>5.5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>130</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31">
+        <v>224</v>
+      </c>
+      <c r="D31">
+        <v>6.5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>131</v>
+      </c>
+      <c r="B32">
+        <v>224</v>
+      </c>
+      <c r="C32">
+        <v>221</v>
+      </c>
+      <c r="D32">
+        <v>5.5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>132</v>
+      </c>
+      <c r="B33">
+        <v>221</v>
+      </c>
+      <c r="C33">
+        <v>218</v>
+      </c>
+      <c r="D33">
+        <v>5.5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>133</v>
+      </c>
+      <c r="B34">
+        <v>218</v>
+      </c>
+      <c r="C34">
+        <v>215</v>
+      </c>
+      <c r="D34">
+        <v>5.5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>134</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>223</v>
+      </c>
+      <c r="D35">
+        <v>6.5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>135</v>
+      </c>
+      <c r="B36">
+        <v>223</v>
+      </c>
+      <c r="C36">
+        <v>220</v>
+      </c>
+      <c r="D36">
+        <v>5.5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" t="s">
+        <v>31</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>136</v>
+      </c>
+      <c r="B37">
+        <v>220</v>
+      </c>
+      <c r="C37">
+        <v>217</v>
+      </c>
+      <c r="D37">
+        <v>5.5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>137</v>
+      </c>
+      <c r="B38">
+        <v>217</v>
+      </c>
+      <c r="C38">
+        <v>214</v>
+      </c>
+      <c r="D38">
+        <v>5.5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>138</v>
+      </c>
+      <c r="B39">
+        <v>212</v>
+      </c>
+      <c r="C39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39">
+        <v>8.5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" t="s">
+        <v>31</v>
+      </c>
+      <c r="G39" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>139</v>
+      </c>
+      <c r="B40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>140</v>
+      </c>
+      <c r="B41" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" t="s">
+        <v>133</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>141</v>
+      </c>
+      <c r="B42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>142</v>
+      </c>
+      <c r="B43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" t="s">
+        <v>135</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>143</v>
+      </c>
+      <c r="B44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" t="s">
+        <v>31</v>
+      </c>
+      <c r="G44" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>144</v>
+      </c>
+      <c r="B45" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" t="s">
+        <v>167</v>
+      </c>
+      <c r="D45">
+        <v>5.5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>145</v>
+      </c>
+      <c r="B46" t="s">
+        <v>138</v>
+      </c>
+      <c r="C46" t="s">
+        <v>166</v>
+      </c>
+      <c r="D46">
+        <v>5.5</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>146</v>
+      </c>
+      <c r="B47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47">
+        <v>5.5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" t="s">
+        <v>31</v>
+      </c>
+      <c r="G47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>147</v>
+      </c>
+      <c r="B48" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48">
+        <v>5.5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>148</v>
+      </c>
+      <c r="B49" t="s">
+        <v>141</v>
+      </c>
+      <c r="C49" t="s">
+        <v>163</v>
+      </c>
+      <c r="D49">
+        <v>5.5</v>
+      </c>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>149</v>
+      </c>
+      <c r="B50" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" t="s">
+        <v>162</v>
+      </c>
+      <c r="D50">
+        <v>5.5</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" t="s">
+        <v>31</v>
+      </c>
+      <c r="G50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>150</v>
+      </c>
+      <c r="B51" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51">
+        <v>3.5</v>
+      </c>
+      <c r="E51" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>151</v>
+      </c>
+      <c r="B52" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" t="s">
+        <v>160</v>
+      </c>
+      <c r="D52">
+        <v>3.5</v>
+      </c>
+      <c r="E52" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" t="s">
+        <v>31</v>
+      </c>
+      <c r="G52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>152</v>
+      </c>
+      <c r="B53" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" t="s">
+        <v>159</v>
+      </c>
+      <c r="D53">
+        <v>3.5</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" t="s">
+        <v>31</v>
+      </c>
+      <c r="G53" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>153</v>
+      </c>
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" t="s">
+        <v>158</v>
+      </c>
+      <c r="D54">
+        <v>3.5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>154</v>
+      </c>
+      <c r="B55" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" t="s">
+        <v>151</v>
+      </c>
+      <c r="D55">
+        <v>5.5</v>
+      </c>
+      <c r="E55" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>155</v>
+      </c>
+      <c r="B56" t="s">
+        <v>152</v>
+      </c>
+      <c r="C56" t="s">
+        <v>153</v>
+      </c>
+      <c r="D56">
+        <v>5.5</v>
+      </c>
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" t="s">
+        <v>31</v>
+      </c>
+      <c r="G56" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>156</v>
+      </c>
+      <c r="B57" t="s">
+        <v>154</v>
+      </c>
+      <c r="C57" t="s">
+        <v>155</v>
+      </c>
+      <c r="D57">
+        <v>5.5</v>
+      </c>
+      <c r="E57" t="s">
+        <v>6</v>
+      </c>
+      <c r="F57" t="s">
+        <v>31</v>
+      </c>
+      <c r="G57" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>157</v>
+      </c>
+      <c r="B58" t="s">
+        <v>156</v>
+      </c>
+      <c r="C58" t="s">
+        <v>157</v>
+      </c>
+      <c r="D58">
+        <v>5.5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G58" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>106</v>
+      </c>
+      <c r="C59" t="s">
+        <v>169</v>
+      </c>
+      <c r="D59">
+        <v>14</v>
+      </c>
+      <c r="G59" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>109</v>
+      </c>
+      <c r="C60" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60">
+        <v>14</v>
+      </c>
+      <c r="G60" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>216</v>
+      </c>
+      <c r="C61" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61">
+        <v>17</v>
+      </c>
+      <c r="G61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>215</v>
+      </c>
+      <c r="C62" t="s">
+        <v>174</v>
+      </c>
+      <c r="D62">
+        <v>17</v>
+      </c>
+      <c r="G62" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>214</v>
+      </c>
+      <c r="C63" t="s">
+        <v>175</v>
+      </c>
+      <c r="D63">
+        <v>17</v>
+      </c>
+      <c r="G63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>238</v>
+      </c>
+      <c r="C64" t="s">
+        <v>176</v>
+      </c>
+      <c r="D64">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
         <v>3</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B67" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
         <v>2</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B68" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1371,7 +2525,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1487,10 +2641,10 @@
         <v>67</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1501,10 +2655,10 @@
         <v>68</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1515,10 +2669,10 @@
         <v>68</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1526,19 +2680,19 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>83</v>
+        <v>168</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1546,19 +2700,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>83</v>
+        <v>168</v>
       </c>
       <c r="C12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F12" t="s">
-        <v>98</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1566,16 +2720,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1583,16 +2737,16 @@
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1600,16 +2754,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C15" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>76</v>
-      </c>
       <c r="E15" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1617,13 +2771,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>67</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1631,13 +2785,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>61</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1645,13 +2799,13 @@
         <v>2</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>67</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1659,16 +2813,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" t="s">
         <v>80</v>
-      </c>
-      <c r="C19" t="s">
-        <v>121</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F19" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1676,27 +2830,27 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1704,13 +2858,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1718,13 +2872,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1732,13 +2886,13 @@
         <v>9</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1746,13 +2900,13 @@
         <v>10</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1760,111 +2914,111 @@
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>107</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
         <v>67</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F31" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D32" t="s">
         <v>67</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F32" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>67</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F33" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1872,16 +3026,16 @@
         <v>13</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D34" t="s">
         <v>67</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>